<commit_message>
read agent init pos
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdai1\GIT\conflict_based_search\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b60e98ec5e6769d/デスクトップ/centralized/mapf/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7E034B-BB54-4B31-9E71-829C94C03384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9C7E034B-BB54-4B31-9E71-829C94C03384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EA38A58-7055-46DE-8403-8DBDEA11052F}"/>
   <bookViews>
-    <workbookView xWindow="-8715" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="agents" sheetId="6" r:id="rId1"/>
@@ -170,7 +170,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>init pos</t>
+    <t>init_pos</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -247,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -514,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DCCC56-748D-4914-82A8-BA4C46386A4E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -554,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ25"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>